<commit_message>
Created figures for each climate zone using python functions for each comparative graph, general code cleanup
</commit_message>
<xml_diff>
--- a/datasets/std100/std100data_percentiles_allclimatezones_allbuildingtypes.xlsx
+++ b/datasets/std100/std100data_percentiles_allclimatezones_allbuildingtypes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\NREL\compare-building-data\datasets\std100\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC673F42-BB14-481D-A8D2-EE4A78A26453}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B07FAB89-D231-4D50-BD1A-0E7801ADC6CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-57720" yWindow="-60" windowWidth="29040" windowHeight="15720" xr2:uid="{BE7DB148-3D7C-475E-9055-E235FB6E8DC7}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{BE7DB148-3D7C-475E-9055-E235FB6E8DC7}"/>
   </bookViews>
   <sheets>
     <sheet name="25thPercentile" sheetId="1" r:id="rId1"/>
@@ -357,9 +357,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1437,21 +1438,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6F136F4-0A8F-4CB5-9064-FFF9996B7581}">
   <dimension ref="A1:V56"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="9" width="4" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.5546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.44140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="22" width="4" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="30.109375" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="4" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultColWidth="14.21875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
@@ -5262,7 +5253,6 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:V56" xr:uid="{C6F136F4-0A8F-4CB5-9064-FFF9996B7581}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
@@ -5273,7 +5263,7 @@
   <dimension ref="A1:V56"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J27" sqref="J27"/>
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9105,8 +9095,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D4E75A4-017C-40AF-A431-7E8AE48093C1}">
   <dimension ref="A1:W56"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="Y19" sqref="Y19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9120,7 +9110,7 @@
     <col min="13" max="23" width="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:23" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
clean up std100 spreadsheet, add readme
</commit_message>
<xml_diff>
--- a/datasets/std100/std100data_percentiles_allclimatezones_allbuildingtypes.xlsx
+++ b/datasets/std100/std100data_percentiles_allclimatezones_allbuildingtypes.xlsx
@@ -1,24 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10608"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\NREL\compare-building-data\datasets\std100\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nlong/working/comstock/compare-building-data/datasets/std100/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B07FAB89-D231-4D50-BD1A-0E7801ADC6CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2B0ACDB-1184-0541-87D7-69B04D8A8E2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{BE7DB148-3D7C-475E-9055-E235FB6E8DC7}"/>
+    <workbookView xWindow="140" yWindow="920" windowWidth="34240" windowHeight="21260" activeTab="2" xr2:uid="{BE7DB148-3D7C-475E-9055-E235FB6E8DC7}"/>
   </bookViews>
   <sheets>
-    <sheet name="25thPercentile" sheetId="1" r:id="rId1"/>
-    <sheet name="40thPercentile" sheetId="4" r:id="rId2"/>
-    <sheet name="50thPercentile" sheetId="6" r:id="rId3"/>
+    <sheet name="site_energy_25th_percentile" sheetId="1" r:id="rId1"/>
+    <sheet name="site_energy_40th_percentile" sheetId="4" r:id="rId2"/>
+    <sheet name="site_energy_50th_percentile" sheetId="6" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'25thPercentile'!$A$1:$V$56</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">site_energy_25th_percentile!$A$1:$V$56</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="92">
   <si>
     <t>No.</t>
   </si>
@@ -315,12 +315,15 @@
   <si>
     <t>Building Category</t>
   </si>
+  <si>
+    <t>site_energy_40th_percentile</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -335,6 +338,13 @@
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF569CD6"/>
+      <name val="Menlo"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -357,10 +367,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -382,16 +393,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>28</xdr:col>
-      <xdr:colOff>428625</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>619125</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>114301</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>32</xdr:col>
-      <xdr:colOff>135255</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>325755</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -406,8 +417,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="12401550" y="0"/>
-          <a:ext cx="2145030" cy="4067175"/>
+          <a:off x="26273125" y="304801"/>
+          <a:ext cx="4024630" cy="1676399"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -498,6 +509,7 @@
             <a:solidFill>
               <a:schemeClr val="dk1"/>
             </a:solidFill>
+            <a:effectLst/>
             <a:latin typeface="+mn-lt"/>
             <a:ea typeface="+mn-ea"/>
             <a:cs typeface="+mn-cs"/>
@@ -508,29 +520,6 @@
             <a:solidFill>
               <a:schemeClr val="dk1"/>
             </a:solidFill>
-            <a:latin typeface="+mn-lt"/>
-            <a:ea typeface="+mn-ea"/>
-            <a:cs typeface="+mn-cs"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-              <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id=""/>
-            </a:rPr>
-            <a:t>https://nrel-my.sharepoint.com/:b:/g/personal/nlong_nrel_gov/EU4leOmcHJpEsSVkcrJnQ5cB_uCSVEnc1-zzRq7mJmPXvA?e=33htYZ</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US" sz="1100">
-            <a:solidFill>
-              <a:schemeClr val="dk1"/>
-            </a:solidFill>
             <a:effectLst/>
             <a:latin typeface="+mn-lt"/>
             <a:ea typeface="+mn-ea"/>
@@ -538,17 +527,23 @@
           </a:endParaRPr>
         </a:p>
         <a:p>
-          <a:endParaRPr lang="en-US" sz="1100" b="0">
-            <a:solidFill>
-              <a:schemeClr val="dk1"/>
-            </a:solidFill>
-            <a:effectLst/>
-            <a:latin typeface="+mn-lt"/>
-            <a:ea typeface="+mn-ea"/>
-            <a:cs typeface="+mn-cs"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
           <a:r>
             <a:rPr lang="en-US" sz="1100" b="0">
               <a:solidFill>
@@ -559,55 +554,18 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>Data represents</a:t>
+            <a:t>Data represents 25th percentile of EUI standards for buildings in different climate zones. </a:t>
           </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t> 25th percentile of EUI standards for buildings in different climate zones</a:t>
-          </a:r>
-          <a:br>
-            <a:rPr lang="en-US" sz="1100" b="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-          </a:br>
-          <a:endParaRPr lang="en-US" sz="1100" b="0" baseline="0">
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
             <a:solidFill>
               <a:schemeClr val="dk1"/>
             </a:solidFill>
-            <a:effectLst/>
             <a:latin typeface="+mn-lt"/>
             <a:ea typeface="+mn-ea"/>
             <a:cs typeface="+mn-cs"/>
           </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>Data represents all climate zones and all building types from source</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US" sz="1100" b="0"/>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -620,16 +578,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>26</xdr:col>
-      <xdr:colOff>76200</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>546100</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>76201</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>32</xdr:col>
-      <xdr:colOff>129540</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>599440</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>177801</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -644,8 +602,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="15925800" y="0"/>
-          <a:ext cx="3714750" cy="2907030"/>
+          <a:off x="10756900" y="266701"/>
+          <a:ext cx="4091940" cy="2387600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -752,30 +710,6 @@
           </a:endParaRPr>
         </a:p>
         <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-              <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id=""/>
-            </a:rPr>
-            <a:t>https://nrel-my.sharepoint.com/:b:/g/personal/nlong_nrel_gov/EU4leOmcHJpEsSVkcrJnQ5cB_uCSVEnc1-zzRq7mJmPXvA?e=33htYZ</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US" sz="1100">
-            <a:solidFill>
-              <a:schemeClr val="dk1"/>
-            </a:solidFill>
-            <a:effectLst/>
-            <a:latin typeface="+mn-lt"/>
-            <a:ea typeface="+mn-ea"/>
-            <a:cs typeface="+mn-cs"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
           <a:endParaRPr lang="en-US" sz="1100" b="0">
             <a:solidFill>
               <a:schemeClr val="dk1"/>
@@ -858,16 +792,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>26</xdr:col>
-      <xdr:colOff>91440</xdr:colOff>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>116840</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>22859</xdr:rowOff>
+      <xdr:rowOff>60959</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>31</xdr:col>
-      <xdr:colOff>129540</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>154940</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -882,8 +816,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="15944850" y="200024"/>
-          <a:ext cx="3086100" cy="3933826"/>
+          <a:off x="11762740" y="251459"/>
+          <a:ext cx="3403600" cy="2631441"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -991,41 +925,6 @@
         </a:p>
         <a:p>
           <a:r>
-            <a:rPr lang="en-US" sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-              <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id=""/>
-            </a:rPr>
-            <a:t>https://nrel-my.sharepoint.com/:b:/g/personal/nlong_nrel_gov/EU4leOmcHJpEsSVkcrJnQ5cB_uCSVEnc1-zzRq7mJmPXvA?e=33htYZ</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US" sz="1100">
-            <a:solidFill>
-              <a:schemeClr val="dk1"/>
-            </a:solidFill>
-            <a:effectLst/>
-            <a:latin typeface="+mn-lt"/>
-            <a:ea typeface="+mn-ea"/>
-            <a:cs typeface="+mn-cs"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="en-US" sz="1100" b="0">
-            <a:solidFill>
-              <a:schemeClr val="dk1"/>
-            </a:solidFill>
-            <a:effectLst/>
-            <a:latin typeface="+mn-lt"/>
-            <a:ea typeface="+mn-ea"/>
-            <a:cs typeface="+mn-cs"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:r>
             <a:rPr lang="en-US" sz="1100" b="0">
               <a:solidFill>
                 <a:schemeClr val="dk1"/>
@@ -1060,31 +959,6 @@
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
           </a:br>
-          <a:endParaRPr lang="en-US" sz="1100" b="0" baseline="0">
-            <a:solidFill>
-              <a:schemeClr val="dk1"/>
-            </a:solidFill>
-            <a:effectLst/>
-            <a:latin typeface="+mn-lt"/>
-            <a:ea typeface="+mn-ea"/>
-            <a:cs typeface="+mn-cs"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>Data represents all climate zones and all building types from source</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
           <a:endParaRPr lang="en-US" sz="1100" b="0" baseline="0">
             <a:solidFill>
               <a:schemeClr val="dk1"/>
@@ -1439,12 +1313,19 @@
   <dimension ref="A1:V56"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.21875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="3.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="9" width="5" customWidth="1"/>
+    <col min="10" max="11" width="8" bestFit="1" customWidth="1"/>
+    <col min="12" max="22" width="5" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1512,7 +1393,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1580,7 +1461,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1648,7 +1529,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1716,7 +1597,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1784,7 +1665,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1852,7 +1733,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1920,7 +1801,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1988,7 +1869,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
@@ -2056,7 +1937,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
@@ -2124,7 +2005,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
@@ -2192,7 +2073,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
@@ -2260,7 +2141,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12</v>
       </c>
@@ -2328,7 +2209,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>13</v>
       </c>
@@ -2396,7 +2277,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>14</v>
       </c>
@@ -2464,7 +2345,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>15</v>
       </c>
@@ -2532,7 +2413,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="17" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>16</v>
       </c>
@@ -2600,7 +2481,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="18" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>17</v>
       </c>
@@ -2668,7 +2549,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="19" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>18</v>
       </c>
@@ -2736,7 +2617,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="20" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>19</v>
       </c>
@@ -2804,7 +2685,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="21" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>20</v>
       </c>
@@ -2872,7 +2753,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="22" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>21</v>
       </c>
@@ -2940,7 +2821,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="23" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>22</v>
       </c>
@@ -3008,7 +2889,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="24" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>23</v>
       </c>
@@ -3076,7 +2957,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="25" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>24</v>
       </c>
@@ -3144,7 +3025,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="26" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>25</v>
       </c>
@@ -3212,7 +3093,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="27" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>26</v>
       </c>
@@ -3280,7 +3161,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="28" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>27</v>
       </c>
@@ -3348,7 +3229,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="29" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>28</v>
       </c>
@@ -3416,7 +3297,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="30" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>29</v>
       </c>
@@ -3484,7 +3365,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="31" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>30</v>
       </c>
@@ -3552,7 +3433,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="32" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>31</v>
       </c>
@@ -3620,7 +3501,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="33" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>32</v>
       </c>
@@ -3688,7 +3569,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="34" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>33</v>
       </c>
@@ -3756,7 +3637,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="35" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>34</v>
       </c>
@@ -3824,7 +3705,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="36" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>35</v>
       </c>
@@ -3892,7 +3773,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="37" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>36</v>
       </c>
@@ -3960,7 +3841,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="38" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>37</v>
       </c>
@@ -4028,7 +3909,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="39" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>38</v>
       </c>
@@ -4096,7 +3977,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="40" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>39</v>
       </c>
@@ -4164,7 +4045,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="41" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>40</v>
       </c>
@@ -4232,7 +4113,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="42" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>41</v>
       </c>
@@ -4300,7 +4181,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="43" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>42</v>
       </c>
@@ -4368,7 +4249,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="44" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>43</v>
       </c>
@@ -4436,7 +4317,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="45" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>44</v>
       </c>
@@ -4504,7 +4385,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="46" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>45</v>
       </c>
@@ -4572,7 +4453,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="47" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>46</v>
       </c>
@@ -4640,7 +4521,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="48" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>47</v>
       </c>
@@ -4708,7 +4589,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="49" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>48</v>
       </c>
@@ -4776,7 +4657,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="50" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>49</v>
       </c>
@@ -4844,7 +4725,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="51" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>50</v>
       </c>
@@ -4912,7 +4793,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="52" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>51</v>
       </c>
@@ -4980,7 +4861,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="53" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>52</v>
       </c>
@@ -5048,7 +4929,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="54" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>53</v>
       </c>
@@ -5116,7 +4997,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="55" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>54</v>
       </c>
@@ -5184,7 +5065,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="56" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>55</v>
       </c>
@@ -5263,21 +5144,20 @@
   <dimension ref="A1:V56"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="L31" sqref="L31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="9" width="4" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.5546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="8.5" bestFit="1" customWidth="1"/>
     <col min="12" max="22" width="4" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="30.109375" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="10.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5345,7 +5225,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -5413,7 +5293,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -5481,7 +5361,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -5549,7 +5429,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -5617,7 +5497,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -5685,7 +5565,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -5753,7 +5633,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -5821,7 +5701,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
@@ -5889,7 +5769,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
@@ -5957,7 +5837,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
@@ -6025,7 +5905,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
@@ -6093,7 +5973,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12</v>
       </c>
@@ -6161,7 +6041,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>13</v>
       </c>
@@ -6229,7 +6109,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>14</v>
       </c>
@@ -6297,7 +6177,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>15</v>
       </c>
@@ -6365,7 +6245,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="17" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>16</v>
       </c>
@@ -6433,7 +6313,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="18" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>17</v>
       </c>
@@ -6501,7 +6381,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="19" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>18</v>
       </c>
@@ -6569,7 +6449,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="20" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>19</v>
       </c>
@@ -6637,7 +6517,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="21" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>20</v>
       </c>
@@ -6705,7 +6585,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="22" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>21</v>
       </c>
@@ -6773,7 +6653,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="23" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>22</v>
       </c>
@@ -6841,7 +6721,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="24" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>23</v>
       </c>
@@ -6909,7 +6789,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="25" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>24</v>
       </c>
@@ -6977,7 +6857,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="26" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>25</v>
       </c>
@@ -7045,7 +6925,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="27" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>26</v>
       </c>
@@ -7113,7 +6993,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="28" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>27</v>
       </c>
@@ -7181,7 +7061,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="29" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>28</v>
       </c>
@@ -7249,7 +7129,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="30" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>29</v>
       </c>
@@ -7317,7 +7197,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="31" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>30</v>
       </c>
@@ -7385,7 +7265,7 @@
         <v>585</v>
       </c>
     </row>
-    <row r="32" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>31</v>
       </c>
@@ -7453,7 +7333,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="33" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>32</v>
       </c>
@@ -7521,7 +7401,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="34" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>33</v>
       </c>
@@ -7589,7 +7469,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="35" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>34</v>
       </c>
@@ -7657,7 +7537,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="36" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>35</v>
       </c>
@@ -7725,7 +7605,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="37" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>36</v>
       </c>
@@ -7793,7 +7673,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="38" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>37</v>
       </c>
@@ -7861,7 +7741,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="39" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>38</v>
       </c>
@@ -7929,7 +7809,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="40" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>39</v>
       </c>
@@ -7997,7 +7877,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="41" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>40</v>
       </c>
@@ -8065,7 +7945,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="42" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>41</v>
       </c>
@@ -8133,7 +8013,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="43" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>42</v>
       </c>
@@ -8201,7 +8081,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="44" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>43</v>
       </c>
@@ -8269,7 +8149,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="45" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>44</v>
       </c>
@@ -8337,7 +8217,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="46" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>45</v>
       </c>
@@ -8405,7 +8285,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="47" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>46</v>
       </c>
@@ -8473,7 +8353,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="48" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>47</v>
       </c>
@@ -8541,7 +8421,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="49" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>48</v>
       </c>
@@ -8609,7 +8489,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="50" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>49</v>
       </c>
@@ -8677,7 +8557,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="51" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>50</v>
       </c>
@@ -8745,7 +8625,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="52" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>51</v>
       </c>
@@ -8813,7 +8693,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="53" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>52</v>
       </c>
@@ -8881,7 +8761,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="54" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>53</v>
       </c>
@@ -8949,7 +8829,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="55" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>54</v>
       </c>
@@ -9017,7 +8897,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="56" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>55</v>
       </c>
@@ -9096,21 +8976,20 @@
   <dimension ref="A1:W56"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L11" sqref="L11"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.21875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.83203125" bestFit="1" customWidth="1"/>
     <col min="4" max="10" width="4" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.5546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="8.5" bestFit="1" customWidth="1"/>
     <col min="13" max="23" width="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:23" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -9181,7 +9060,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -9252,7 +9131,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -9323,7 +9202,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -9394,7 +9273,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -9465,7 +9344,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -9536,7 +9415,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -9607,7 +9486,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -9678,7 +9557,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
@@ -9749,7 +9628,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
@@ -9820,7 +9699,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
@@ -9891,7 +9770,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
@@ -9962,7 +9841,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12</v>
       </c>
@@ -10033,7 +9912,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>13</v>
       </c>
@@ -10104,7 +9983,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>14</v>
       </c>
@@ -10175,9 +10054,9 @@
         <v>98</v>
       </c>
     </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A16">
-        <v>15</v>
+    <row r="16" spans="1:23" ht="16" x14ac:dyDescent="0.2">
+      <c r="A16" s="3" t="s">
+        <v>91</v>
       </c>
       <c r="B16" t="s">
         <v>88</v>
@@ -10246,7 +10125,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="17" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>16</v>
       </c>
@@ -10317,7 +10196,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="18" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>17</v>
       </c>
@@ -10388,7 +10267,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="19" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>18</v>
       </c>
@@ -10459,7 +10338,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="20" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>19</v>
       </c>
@@ -10530,7 +10409,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="21" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>20</v>
       </c>
@@ -10601,7 +10480,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="22" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>21</v>
       </c>
@@ -10672,7 +10551,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="23" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>22</v>
       </c>
@@ -10743,7 +10622,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="24" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>23</v>
       </c>
@@ -10814,7 +10693,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="25" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>24</v>
       </c>
@@ -10885,7 +10764,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="26" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>25</v>
       </c>
@@ -10956,7 +10835,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="27" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>26</v>
       </c>
@@ -11027,7 +10906,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="28" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>27</v>
       </c>
@@ -11098,7 +10977,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="29" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>28</v>
       </c>
@@ -11169,7 +11048,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="30" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>29</v>
       </c>
@@ -11240,7 +11119,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="31" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>30</v>
       </c>
@@ -11311,7 +11190,7 @@
         <v>688</v>
       </c>
     </row>
-    <row r="32" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>31</v>
       </c>
@@ -11382,7 +11261,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="33" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>32</v>
       </c>
@@ -11453,7 +11332,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="34" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>33</v>
       </c>
@@ -11524,7 +11403,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="35" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>34</v>
       </c>
@@ -11595,7 +11474,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="36" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>35</v>
       </c>
@@ -11666,7 +11545,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="37" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>36</v>
       </c>
@@ -11737,7 +11616,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="38" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>37</v>
       </c>
@@ -11808,7 +11687,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="39" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>38</v>
       </c>
@@ -11879,7 +11758,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="40" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>39</v>
       </c>
@@ -11950,7 +11829,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="41" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>40</v>
       </c>
@@ -12021,7 +11900,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="42" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>41</v>
       </c>
@@ -12092,7 +11971,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="43" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>42</v>
       </c>
@@ -12163,7 +12042,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="44" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>43</v>
       </c>
@@ -12234,7 +12113,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="45" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>44</v>
       </c>
@@ -12305,7 +12184,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="46" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>45</v>
       </c>
@@ -12376,7 +12255,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="47" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>46</v>
       </c>
@@ -12447,7 +12326,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="48" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>47</v>
       </c>
@@ -12518,7 +12397,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="49" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>48</v>
       </c>
@@ -12589,7 +12468,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="50" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>49</v>
       </c>
@@ -12660,7 +12539,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="51" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>50</v>
       </c>
@@ -12731,7 +12610,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="52" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>51</v>
       </c>
@@ -12802,7 +12681,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="53" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>52</v>
       </c>
@@ -12873,7 +12752,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="54" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>53</v>
       </c>
@@ -12944,7 +12823,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="55" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>54</v>
       </c>
@@ -13015,7 +12894,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="56" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>55</v>
       </c>
@@ -13090,4 +12969,10 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
+<clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
+  <clbl:label id="{95965d95-ecc0-4720-b759-1f33c42ed7da}" enabled="1" method="Standard" siteId="{a0f29d7e-28cd-4f54-8442-7885aee7c080}" contentBits="0" removed="0"/>
+</clbl:labelList>
 </file>
</xml_diff>